<commit_message>
Finished July 2025 Sulfide QAQC for individual plates
</commit_message>
<xml_diff>
--- a/Porewater/Sulfide/Synoptic_CB/2025/July/Raw Data/2025July_H2S_Datasheets.xlsx
+++ b/Porewater/Sulfide/Synoptic_CB/2025/July/Raw Data/2025July_H2S_Datasheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/readz_si_edu1/Documents/synoptic-discrete-data/Porewater/Sulfide/Synoptic_CB/2025/July/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="350" documentId="13_ncr:1_{92021526-6563-4582-BD6D-EF31E3B89D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE08D7AA-FE3E-4852-AE83-473EDE895C60}"/>
+  <xr:revisionPtr revIDLastSave="352" documentId="13_ncr:1_{92021526-6563-4582-BD6D-EF31E3B89D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0528B180-5BFF-4E31-B768-ADED79FD090D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{23FB6DB2-3641-4E78-A68E-113D11F8B05A}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{23FB6DB2-3641-4E78-A68E-113D11F8B05A}"/>
   </bookViews>
   <sheets>
     <sheet name="STD" sheetId="1" r:id="rId1"/>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A61B9A-122A-4013-9523-6CC5BC911E04}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1921,8 +1921,12 @@
       <c r="E2" s="5">
         <v>15</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="5">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5">
+        <v>15</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1946,8 +1950,12 @@
       <c r="E3" s="5">
         <v>18</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="F3" s="5">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5">
+        <v>18</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1972,8 +1980,12 @@
       <c r="E4" s="5">
         <v>43</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="5">
+        <v>43</v>
+      </c>
+      <c r="G4" s="5">
+        <v>43</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2160,8 +2172,12 @@
       <c r="E12" s="4">
         <v>250</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="4">
+        <v>250</v>
+      </c>
+      <c r="G12" s="4">
+        <v>250</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -2185,8 +2201,12 @@
       <c r="E13" s="4">
         <v>250</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="4">
+        <v>250</v>
+      </c>
+      <c r="G13" s="4">
+        <v>250</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -2210,8 +2230,12 @@
       <c r="E14" s="4">
         <v>50</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="F14" s="4">
+        <v>50</v>
+      </c>
+      <c r="G14" s="4">
+        <v>50</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -6699,7 +6723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA7A128-AAAB-4C49-ACE5-ABC21CC91650}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>

</xml_diff>